<commit_message>
Updated sheet names in consolidated xlsx file, and updated RQ2 scripts accordingly
</commit_message>
<xml_diff>
--- a/Analysis_and_Visualization/data/data.xlsx
+++ b/Analysis_and_Visualization/data/data.xlsx
@@ -8,17 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\research\2026-SLR-regression-testing-optimization\Analysis_and_Visualization\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7345AA4-5788-4944-989D-FB8E23EB7D86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ED3C1B6-BEB9-4651-AB7D-64CFD72E2A68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="2" activeTab="4" xr2:uid="{FF880EED-EA60-9E49-B15D-179496B980D1}"/>
+    <workbookView xWindow="-23148" yWindow="1344" windowWidth="23256" windowHeight="13896" firstSheet="4" activeTab="6" xr2:uid="{FF880EED-EA60-9E49-B15D-179496B980D1}"/>
   </bookViews>
   <sheets>
     <sheet name="data_extraction" sheetId="2" r:id="rId1"/>
-    <sheet name="RQ1_trends_by_category_per_year" sheetId="3" r:id="rId2"/>
-    <sheet name="RQ1_replicability_per_year" sheetId="5" r:id="rId3"/>
-    <sheet name="p_taxonomy_vs_algorithm" sheetId="4" r:id="rId4"/>
-    <sheet name="s_taxonomy_vs_algorithm" sheetId="6" r:id="rId5"/>
-    <sheet name="raw_data" sheetId="1" r:id="rId6"/>
+    <sheet name="Sheet2" sheetId="7" r:id="rId2"/>
+    <sheet name="RQ1_trends_by_category_per_year" sheetId="3" r:id="rId3"/>
+    <sheet name="RQ1_replicability_per_year" sheetId="5" r:id="rId4"/>
+    <sheet name="RQ2_p_taxonomy_vs_algorithm" sheetId="4" r:id="rId5"/>
+    <sheet name="RQ2_s_taxonomy_vs_algorithm" sheetId="6" r:id="rId6"/>
+    <sheet name="RQ3_datasets" sheetId="8" r:id="rId7"/>
+    <sheet name="raw_data" sheetId="1" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -63,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4013" uniqueCount="1414">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4036" uniqueCount="1419">
   <si>
     <t>ID</t>
   </si>
@@ -4516,6 +4518,21 @@
   </si>
   <si>
     <t>Full Replication</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>Dataset</t>
+  </si>
+  <si>
+    <t>Industrial/Proprietary</t>
+  </si>
+  <si>
+    <t>Apache Projects</t>
   </si>
 </sst>
 </file>
@@ -19598,6 +19615,18 @@
 </table>
 </file>
 
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{60427D65-C1BB-4033-B0DD-E94497FE33A0}" name="Table6" displayName="Table6" ref="A1:C11" totalsRowShown="0">
+  <autoFilter ref="A1:C11" xr:uid="{60427D65-C1BB-4033-B0DD-E94497FE33A0}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{753159F4-E1F4-4C7F-B96C-8F83BFFE0C97}" name="Category"/>
+    <tableColumn id="2" xr3:uid="{0FC65BCC-69FC-4BB2-9DAB-17504311DCEC}" name="Dataset"/>
+    <tableColumn id="3" xr3:uid="{CA0BB715-AB2B-45E1-BD50-EC4A32F5B80B}" name="Count"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -19917,8 +19946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B91C968-CFFD-1A41-862E-46C430B19788}">
   <dimension ref="A1:AI126"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B34"/>
+    <sheetView topLeftCell="O30" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AD69" sqref="AD69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -27279,6 +27308,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3303011-4926-48DA-9FA6-CCECBB8AE073}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1390148-23A2-4193-A1D6-FE2CB6ADD788}">
   <dimension ref="A1:E15"/>
   <sheetViews>
@@ -27559,7 +27600,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1A6ACA0-5BAF-4CF3-A9BA-46A30A6E0A57}">
   <dimension ref="A1:D14"/>
   <sheetViews>
@@ -27773,7 +27814,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86AC6C15-2C38-4F0A-BF61-EE73FED61ED7}">
   <dimension ref="A1:G11"/>
   <sheetViews>
@@ -28053,11 +28094,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8F05C8F-316F-4046-A284-28124FE5A655}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5:G5"/>
     </sheetView>
   </sheetViews>
@@ -28194,12 +28235,157 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81EB23CA-A17F-4A62-9AC4-DA1175EB60E4}">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6"/>
+  <cols>
+    <col min="1" max="1" width="10.69921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>1414</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1416</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1415</v>
+      </c>
+      <c r="E1" s="37"/>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>1051</v>
+      </c>
+      <c r="B2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>1051</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1404</v>
+      </c>
+      <c r="C3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>1051</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1418</v>
+      </c>
+      <c r="C4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>1051</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1417</v>
+      </c>
+      <c r="C5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>1051</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1407</v>
+      </c>
+      <c r="C6">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1404</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1418</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1417</v>
+      </c>
+      <c r="C10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1407</v>
+      </c>
+      <c r="C11">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BA3DE9A-9DC8-9B4C-920E-613E1AA78E62}">
   <dimension ref="A1:HM126"/>
   <sheetViews>
-    <sheetView topLeftCell="AV1" zoomScale="71" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="BH1" sqref="BH1:BN12"/>
+    <sheetView topLeftCell="AD1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="AF4" sqref="AF4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>

</xml_diff>